<commit_message>
made variable declerations in BoardCell cleaner
</commit_message>
<xml_diff>
--- a/data/ClueLayout306.xlsx
+++ b/data/ClueLayout306.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/170d6889d8d02b02/Documents_1D/Education/_Mines/CSCI306/Classes/Clue Material/Clue Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyno\CSCI306\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1218" documentId="8_{9B645E34-7536-42D9-BF6C-9EF036B3BE1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C89964C2-8466-4C0D-8A88-08D786A93F46}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C57B3CD-768D-4234-85AA-44AC893D878A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="1740" windowWidth="16695" windowHeight="13260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" ClueLayout" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="csv" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="46">
   <si>
     <t>C</t>
   </si>
@@ -157,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -3514,8 +3518,8 @@
       <c r="Y2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="3">
-        <v>0</v>
+      <c r="Z2" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="AB2" s="19" t="s">
         <v>42</v>

</xml_diff>